<commit_message>
make API key and email credentials external
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexeyks/coding/OOP_python/app7-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexeyks/coding/OOP_python/NewsMailSender/NewsMailSender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DD506C-B76E-EF4B-A601-51ADA3FEF413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467913B-61CF-3843-A9A7-84A1131A989D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15960" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -43,23 +43,35 @@
     <t>Marry</t>
   </si>
   <si>
-    <t>g2y3jce4@freeml.net</t>
-  </si>
-  <si>
-    <t>afaqozilw@yomail.info</t>
-  </si>
-  <si>
     <t>Cyprus</t>
   </si>
   <si>
     <t>Cycle</t>
+  </si>
+  <si>
+    <t>g369keh0@freeml.net</t>
+  </si>
+  <si>
+    <t>rndgmvkcf@emlpro.com</t>
+  </si>
+  <si>
+    <t>Kira</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>karzanovalexey@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -70,6 +82,20 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -312,12 +338,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -375,8 +404,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1541,7 +1580,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1577,10 +1616,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" s="7"/>
     </row>
@@ -1592,18 +1631,26 @@
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="14.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1649,6 +1696,9 @@
       <c r="E10" s="18"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{8F6E701C-6250-564C-98DE-FEA58B9504BB}"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>

</xml_diff>

<commit_message>
add error handling, change email template, add logging and unit testing
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexeyks/coding/OOP_python/NewsMailSender/NewsMailSender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467913B-61CF-3843-A9A7-84A1131A989D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5A5564-4520-4F49-B057-CC35E0BD589E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15960" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>